<commit_message>
se agrego el trabajo con la fecha automatico y manejo de numero de actividades
</commit_message>
<xml_diff>
--- a/planes/media/anexos/Arquitectura_de_Redes.xlsx
+++ b/planes/media/anexos/Arquitectura_de_Redes.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Carlos\Documents\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8F21064A-AC84-4BFB-BC1A-C9EAC3E8CACC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B02086D6-3F74-4647-BB4E-39AA0DA04D9D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11040" xr2:uid="{CFEC9D7A-85E0-4CDB-9ECA-7617E874903D}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="55" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="24">
   <si>
     <t>Docente</t>
   </si>
@@ -59,21 +59,12 @@
     <t>Trabajo Independiente</t>
   </si>
   <si>
-    <t>Redes y Telecomunicaciones</t>
-  </si>
-  <si>
-    <t>Primero</t>
-  </si>
-  <si>
     <t>Encuadre</t>
   </si>
   <si>
     <t>Firmar Encuadre</t>
   </si>
   <si>
-    <t>Ing. Carlos Guzmán</t>
-  </si>
-  <si>
     <t>Prueba Diagnóstico</t>
   </si>
   <si>
@@ -107,7 +98,16 @@
     <t>Manual de reparación</t>
   </si>
   <si>
-    <t>Arquitectura de Redes</t>
+    <t>Ing. Carlos Guzman</t>
+  </si>
+  <si>
+    <t>ARQUITECTURA DE REDES</t>
+  </si>
+  <si>
+    <t>SEGUNDO</t>
+  </si>
+  <si>
+    <t>REDES Y TELECOMUNICACIONES</t>
   </si>
 </sst>
 </file>
@@ -505,10 +505,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{77D00BB1-5F2C-4271-B6A3-A111FE818A73}">
-  <dimension ref="A1:G9"/>
+  <dimension ref="A1:G19"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B2" sqref="B2:B9"/>
+      <selection activeCell="I14" sqref="I14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -545,186 +545,416 @@
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B2" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C2" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="D2" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="F2" t="s">
-        <v>9</v>
+        <v>7</v>
       </c>
       <c r="G2" t="s">
-        <v>10</v>
+        <v>8</v>
       </c>
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B3" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C3" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="D3" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="E3">
         <v>2</v>
       </c>
       <c r="F3" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="G3" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B4" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C4" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="D4" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="E4">
         <v>3</v>
       </c>
       <c r="F4" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="G4" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B5" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C5" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="D5" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="E5">
         <v>4</v>
       </c>
       <c r="F5" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="G5" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B6" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C6" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="D6" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="E6">
         <v>5</v>
       </c>
       <c r="F6" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="G6" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B7" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="D7" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="E7">
         <v>6</v>
       </c>
       <c r="F7" t="s">
+        <v>16</v>
+      </c>
+      <c r="G7" t="s">
         <v>19</v>
-      </c>
-      <c r="G7" t="s">
-        <v>22</v>
       </c>
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B8" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C8" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="D8" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="E8">
         <v>7</v>
       </c>
       <c r="F8" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="G8" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
-        <v>11</v>
+        <v>20</v>
       </c>
       <c r="B9" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="C9" t="s">
-        <v>7</v>
+        <v>23</v>
       </c>
       <c r="D9" t="s">
-        <v>8</v>
+        <v>22</v>
       </c>
       <c r="E9">
         <v>8</v>
       </c>
       <c r="F9" t="s">
+        <v>12</v>
+      </c>
+      <c r="G9" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A10" t="s">
+        <v>20</v>
+      </c>
+      <c r="B10" t="s">
+        <v>21</v>
+      </c>
+      <c r="C10" t="s">
+        <v>23</v>
+      </c>
+      <c r="D10" t="s">
+        <v>22</v>
+      </c>
+      <c r="E10">
+        <v>9</v>
+      </c>
+      <c r="F10" t="s">
+        <v>7</v>
+      </c>
+      <c r="G10" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A11" t="s">
+        <v>20</v>
+      </c>
+      <c r="B11" t="s">
+        <v>21</v>
+      </c>
+      <c r="C11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" t="s">
+        <v>22</v>
+      </c>
+      <c r="E11">
+        <v>10</v>
+      </c>
+      <c r="F11" t="s">
+        <v>9</v>
+      </c>
+      <c r="G11" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A12" t="s">
+        <v>20</v>
+      </c>
+      <c r="B12" t="s">
+        <v>21</v>
+      </c>
+      <c r="C12" t="s">
+        <v>23</v>
+      </c>
+      <c r="D12" t="s">
+        <v>22</v>
+      </c>
+      <c r="E12">
+        <v>11</v>
+      </c>
+      <c r="F12" t="s">
+        <v>11</v>
+      </c>
+      <c r="G12" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A13" t="s">
+        <v>20</v>
+      </c>
+      <c r="B13" t="s">
+        <v>21</v>
+      </c>
+      <c r="C13" t="s">
+        <v>23</v>
+      </c>
+      <c r="D13" t="s">
+        <v>22</v>
+      </c>
+      <c r="E13">
+        <v>12</v>
+      </c>
+      <c r="F13" t="s">
+        <v>13</v>
+      </c>
+      <c r="G13" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A14" t="s">
+        <v>20</v>
+      </c>
+      <c r="B14" t="s">
+        <v>21</v>
+      </c>
+      <c r="C14" t="s">
+        <v>23</v>
+      </c>
+      <c r="D14" t="s">
+        <v>22</v>
+      </c>
+      <c r="E14">
+        <v>13</v>
+      </c>
+      <c r="F14" t="s">
         <v>15</v>
       </c>
-      <c r="G9" t="s">
-        <v>13</v>
+      <c r="G14" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A15" t="s">
+        <v>20</v>
+      </c>
+      <c r="B15" t="s">
+        <v>21</v>
+      </c>
+      <c r="C15" t="s">
+        <v>23</v>
+      </c>
+      <c r="D15" t="s">
+        <v>22</v>
+      </c>
+      <c r="E15">
+        <v>14</v>
+      </c>
+      <c r="F15" t="s">
+        <v>16</v>
+      </c>
+      <c r="G15" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>20</v>
+      </c>
+      <c r="B16" t="s">
+        <v>21</v>
+      </c>
+      <c r="C16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" t="s">
+        <v>22</v>
+      </c>
+      <c r="E16">
+        <v>15</v>
+      </c>
+      <c r="F16" t="s">
+        <v>17</v>
+      </c>
+      <c r="G16" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="17" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>20</v>
+      </c>
+      <c r="B17" t="s">
+        <v>21</v>
+      </c>
+      <c r="C17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D17" t="s">
+        <v>22</v>
+      </c>
+      <c r="E17">
+        <v>16</v>
+      </c>
+      <c r="F17" t="s">
+        <v>7</v>
+      </c>
+      <c r="G17" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="18" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>20</v>
+      </c>
+      <c r="B18" t="s">
+        <v>21</v>
+      </c>
+      <c r="C18" t="s">
+        <v>23</v>
+      </c>
+      <c r="D18" t="s">
+        <v>22</v>
+      </c>
+      <c r="E18">
+        <v>17</v>
+      </c>
+      <c r="F18" t="s">
+        <v>9</v>
+      </c>
+      <c r="G18" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="19" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="A19" t="s">
+        <v>20</v>
+      </c>
+      <c r="B19" t="s">
+        <v>21</v>
+      </c>
+      <c r="C19" t="s">
+        <v>23</v>
+      </c>
+      <c r="D19" t="s">
+        <v>22</v>
+      </c>
+      <c r="E19">
+        <v>18</v>
+      </c>
+      <c r="F19" t="s">
+        <v>7</v>
+      </c>
+      <c r="G19" t="s">
+        <v>8</v>
       </c>
     </row>
   </sheetData>

</xml_diff>